<commit_message>
add the CSV versions of the xl as well as the corr
</commit_message>
<xml_diff>
--- a/EXPECTED_COST.xlsx
+++ b/EXPECTED_COST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Desktop\Git Projects\portfolio-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FC4C5E-9F1F-4191-B675-E858B50D68BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD43BE5-0C58-49B2-8B1B-F853223BF40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5267E136-FC7F-456F-BD2C-5678260828EA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5267E136-FC7F-456F-BD2C-5678260828EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1853,7 +1853,7 @@
   <dimension ref="A1:E1925"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E1925"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>